<commit_message>
scrum file aktualisiert: backlogID, sprint
</commit_message>
<xml_diff>
--- a/doc/task04/SED_ProductPlaningMeeting_scrum_v02.xlsx
+++ b/doc/task04/SED_ProductPlaningMeeting_scrum_v02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Denis\git\ch.bfh.btx8081.w2020.red\doc\task04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFCFA7F0-8495-4024-8715-F56887104367}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D330BDF-F634-4E14-8BFB-DBC53C6A3F81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -856,7 +856,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,22 +904,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>89</v>
+        <v>17</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="I2" s="6">
-        <v>44149</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -927,20 +924,21 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:9" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -1153,7 +1151,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1212,7 +1210,7 @@
     </row>
     <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1.1000000000000001</v>
+        <v>1.01</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1243,7 +1241,7 @@
       </c>
       <c r="K2">
         <f>SUM(K3:K10)</f>
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="L2" t="s">
         <v>9</v>
@@ -1251,7 +1249,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1.2</v>
+        <v>1.02</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1284,12 +1282,12 @@
         <v>3</v>
       </c>
       <c r="L3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1.3</v>
+        <v>1.03</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1324,7 +1322,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1.4</v>
+        <v>1.04</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1354,15 +1352,15 @@
         <v>92</v>
       </c>
       <c r="K5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1.5</v>
+        <v>1.05</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1395,12 +1393,12 @@
         <v>3</v>
       </c>
       <c r="L6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>1.6</v>
+        <v>1.06</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1438,7 +1436,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1.7</v>
+        <v>1.07</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1468,15 +1466,15 @@
         <v>92</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1.8</v>
+        <v>1.08</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1514,7 +1512,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1.9</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1547,12 +1545,12 @@
         <v>0</v>
       </c>
       <c r="L10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1598,7 +1596,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A3" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Sprint 2 angefangen zu planen
</commit_message>
<xml_diff>
--- a/doc/task04/SED_ProductPlaningMeeting_scrum_v02.xlsx
+++ b/doc/task04/SED_ProductPlaningMeeting_scrum_v02.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sibcode/IdeaProjects/ch.bfh.btx8081.w2020.red/doc/task04/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Denis\git\ch.bfh.btx8081.w2020.red\doc\task04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{496E517C-4641-CE49-8617-D07624C0B7A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19397155-62DD-4CA5-8E1F-D7C3F47715AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="124">
   <si>
     <t>ID</t>
   </si>
@@ -389,13 +389,40 @@
   </si>
   <si>
     <t xml:space="preserve">Login-View </t>
+  </si>
+  <si>
+    <t>Instructionen Erstellen</t>
+  </si>
+  <si>
+    <t>Implementieren Instruction View</t>
+  </si>
+  <si>
+    <t>Implementieren Add Instruction View</t>
+  </si>
+  <si>
+    <t>Implementierung Instruction Model</t>
+  </si>
+  <si>
+    <t>Einrichten SQLite</t>
+  </si>
+  <si>
+    <t>SQLite</t>
+  </si>
+  <si>
+    <t>Persistierung einrichten</t>
+  </si>
+  <si>
+    <t>Instruction Model</t>
+  </si>
+  <si>
+    <t>56?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -407,6 +434,13 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -444,7 +478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -462,9 +496,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -480,7 +515,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -806,13 +841,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="2" width="26.83203125" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="2" customFormat="1" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -820,7 +855,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>81</v>
       </c>
@@ -828,7 +863,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -836,7 +871,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>83</v>
       </c>
@@ -844,7 +879,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>84</v>
       </c>
@@ -862,24 +897,24 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="22" style="1" customWidth="1"/>
     <col min="3" max="3" width="71" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.1640625" style="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -905,7 +940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -925,7 +960,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -946,7 +981,7 @@
       </c>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:9" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -966,7 +1001,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -986,7 +1021,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1006,7 +1041,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1026,7 +1061,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1046,7 +1081,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1066,7 +1101,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1086,7 +1121,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1106,7 +1141,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1126,7 +1161,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1154,29 +1189,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="I15" sqref="I14:I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="19.5" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" customWidth="1"/>
-    <col min="9" max="9" width="7.83203125" customWidth="1"/>
-    <col min="10" max="10" width="9.1640625" customWidth="1"/>
-    <col min="11" max="11" width="7.33203125" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1214,7 +1249,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.01</v>
       </c>
@@ -1253,7 +1288,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1.02</v>
       </c>
@@ -1291,7 +1326,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1.03</v>
       </c>
@@ -1326,7 +1361,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1.04</v>
       </c>
@@ -1364,7 +1399,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1.05</v>
       </c>
@@ -1402,7 +1437,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1.06</v>
       </c>
@@ -1440,7 +1475,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1.07</v>
       </c>
@@ -1478,7 +1513,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1.08</v>
       </c>
@@ -1516,7 +1551,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1.0900000000000001</v>
       </c>
@@ -1554,7 +1589,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1.1000000000000001</v>
       </c>
@@ -1592,9 +1627,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>1.1000000000000001</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1625,6 +1660,257 @@
       </c>
       <c r="L12" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5.01</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>115</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1.07</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" t="s">
+        <v>105</v>
+      </c>
+      <c r="F14" t="s">
+        <v>96</v>
+      </c>
+      <c r="G14" t="s">
+        <v>93</v>
+      </c>
+      <c r="H14" t="s">
+        <v>5</v>
+      </c>
+      <c r="J14" t="s">
+        <v>92</v>
+      </c>
+      <c r="L14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" t="s">
+        <v>114</v>
+      </c>
+      <c r="E15" t="s">
+        <v>104</v>
+      </c>
+      <c r="F15" t="s">
+        <v>93</v>
+      </c>
+      <c r="G15" t="s">
+        <v>99</v>
+      </c>
+      <c r="H15" t="s">
+        <v>5</v>
+      </c>
+      <c r="L15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>119</v>
+      </c>
+      <c r="D16" t="s">
+        <v>121</v>
+      </c>
+      <c r="E16" t="s">
+        <v>120</v>
+      </c>
+      <c r="F16" t="s">
+        <v>96</v>
+      </c>
+      <c r="G16" t="s">
+        <v>99</v>
+      </c>
+      <c r="H16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>5.03</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>119</v>
+      </c>
+      <c r="D17" t="s">
+        <v>121</v>
+      </c>
+      <c r="E17" t="s">
+        <v>120</v>
+      </c>
+      <c r="F17" t="s">
+        <v>95</v>
+      </c>
+      <c r="G17" t="s">
+        <v>99</v>
+      </c>
+      <c r="H17" t="s">
+        <v>5</v>
+      </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>5.04</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>119</v>
+      </c>
+      <c r="D18" t="s">
+        <v>121</v>
+      </c>
+      <c r="E18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F18" t="s">
+        <v>97</v>
+      </c>
+      <c r="G18" t="s">
+        <v>99</v>
+      </c>
+      <c r="H18" t="s">
+        <v>5</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>119</v>
+      </c>
+      <c r="D19" t="s">
+        <v>121</v>
+      </c>
+      <c r="E19" t="s">
+        <v>120</v>
+      </c>
+      <c r="F19" t="s">
+        <v>93</v>
+      </c>
+      <c r="G19" t="s">
+        <v>99</v>
+      </c>
+      <c r="H19" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" t="s">
+        <v>107</v>
+      </c>
+      <c r="E20" t="s">
+        <v>104</v>
+      </c>
+      <c r="F20" t="s">
+        <v>95</v>
+      </c>
+      <c r="G20" t="s">
+        <v>99</v>
+      </c>
+      <c r="H20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>117</v>
+      </c>
+      <c r="D21" t="s">
+        <v>107</v>
+      </c>
+      <c r="E21" t="s">
+        <v>104</v>
+      </c>
+      <c r="F21" t="s">
+        <v>95</v>
+      </c>
+      <c r="G21" t="s">
+        <v>99</v>
+      </c>
+      <c r="H21" t="s">
+        <v>5</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>118</v>
+      </c>
+      <c r="D22" t="s">
+        <v>122</v>
+      </c>
+      <c r="I22">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1640,14 +1926,14 @@
       <selection activeCell="A3" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>44</v>
       </c>
@@ -1661,7 +1947,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1675,7 +1961,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1703,20 +1989,20 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="22" style="1" customWidth="1"/>
-    <col min="3" max="3" width="31.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1640625" style="1"/>
+    <col min="3" max="3" width="31.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1742,7 +2028,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1768,7 +2054,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1785,7 +2071,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1802,7 +2088,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1833,20 +2119,20 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="22" style="1" customWidth="1"/>
     <col min="3" max="3" width="71" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1640625" style="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1872,7 +2158,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1895,7 +2181,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1912,7 +2198,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1935,7 +2221,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1958,7 +2244,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1981,7 +2267,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1998,7 +2284,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2015,7 +2301,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>66</v>
       </c>
@@ -2026,7 +2312,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="245.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="245.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -2040,7 +2326,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="165" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="165" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -2051,7 +2337,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -2059,22 +2345,22 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -2093,20 +2379,20 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="22" style="1" customWidth="1"/>
     <col min="3" max="3" width="71" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1640625" style="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2132,7 +2418,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2155,7 +2441,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2172,7 +2458,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2195,7 +2481,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2218,7 +2504,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2241,7 +2527,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2258,7 +2544,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2275,7 +2561,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>66</v>
       </c>
@@ -2286,7 +2572,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="245.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="245.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -2300,7 +2586,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="165" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="165" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -2311,7 +2597,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -2319,22 +2605,22 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -2353,23 +2639,23 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="19.5" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" customWidth="1"/>
-    <col min="9" max="9" width="7.83203125" customWidth="1"/>
-    <col min="10" max="10" width="9.1640625" customWidth="1"/>
-    <col min="11" max="11" width="7.33203125" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2407,7 +2693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="64" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1.1000000000000001</v>
       </c>
@@ -2445,7 +2731,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1.2</v>
       </c>
@@ -2477,7 +2763,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1.3</v>
       </c>
@@ -2510,7 +2796,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2.1</v>
       </c>
@@ -2542,7 +2828,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2.2000000000000002</v>
       </c>
@@ -2587,14 +2873,14 @@
       <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>44</v>
       </c>
@@ -2608,7 +2894,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2622,7 +2908,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>

</xml_diff>